<commit_message>
Grades, Subjects Reading, Grades writting
</commit_message>
<xml_diff>
--- a/grades.xlsx
+++ b/grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wes_b\progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B875D69-2322-4737-8429-CACA3EC2B5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77F7E39-2FEE-4F4F-BF65-6202ADC356F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <t>mark</t>
   </si>
   <si>
-    <t>grade_id</t>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>